<commit_message>
SM : ajout CSV pour Marc
</commit_message>
<xml_diff>
--- a/public/files/modele_import_sm_v1.xlsx
+++ b/public/files/modele_import_sm_v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Modele import Smartphones reconditionneur pro (format xls)</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Catégorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erreur</t>
   </si>
 </sst>
 </file>
@@ -300,10 +303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -378,6 +381,9 @@
       </c>
       <c r="T2" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>